<commit_message>
Stage 보상 api 추가
버그 확인 필요
</commit_message>
<xml_diff>
--- a/Data/Excel/Model/User/World.xlsx
+++ b/Data/Excel/Model/User/World.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Model\User\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774A678B-A958-4D2E-B6F7-616977400A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B2C051-C143-4AD3-9378-638D3E8A65B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -82,11 +82,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Order</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>Flag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TopFinishStageOrder</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RecvStarReward</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1021,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1085,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1089,7 +1093,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1097,7 +1101,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1105,17 +1109,25 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>